<commit_message>
Nueva Wallet Purchase Order Amazon
</commit_message>
<xml_diff>
--- a/WRRDEI24.xlsx
+++ b/WRRDEI24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qvile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qvile\Desktop\Wallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC03701D-0605-4032-8641-3A58B96C0D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040FB42D-5E78-4130-B16F-9EC8A17452F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{107A0EE1-797D-45B4-A040-8CCE78027CD2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Ingrés</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>Saldo 18/12/2024</t>
+  </si>
+  <si>
+    <t>Saldo 21/12/2024</t>
+  </si>
+  <si>
+    <t>Norton Soft</t>
+  </si>
+  <si>
+    <t>SongSterr</t>
+  </si>
+  <si>
+    <t>Amazon DEL</t>
+  </si>
+  <si>
+    <t>Brilliant</t>
+  </si>
+  <si>
+    <t>Amazon PO241884</t>
   </si>
 </sst>
 </file>
@@ -364,7 +382,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
@@ -612,11 +649,88 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="$B$29">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo: una sola esquina cortada 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F36706B8-1E1D-479F-8354-BE65F1FD4F60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127000" y="5245100"/>
+          <a:ext cx="2654300" cy="774700"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:fld id="{130FBDAF-7E87-41ED-A456-0FFE7A32E210}" type="TxLink">
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:t>Saldo: -214,05 €</a:t>
+          </a:fld>
+          <a:endParaRPr lang="es-ES" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Aptos Narrow"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4537701E-1A22-4956-90E8-02D8F215B27D}" name="Tabla1" displayName="Tabla1" ref="B2:C7" totalsRowCount="1" headerRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4537701E-1A22-4956-90E8-02D8F215B27D}" name="Tabla1" displayName="Tabla1" ref="B2:C7" totalsRowCount="1" headerRowBorderDxfId="21">
   <autoFilter ref="B2:C6" xr:uid="{4537701E-1A22-4956-90E8-02D8F215B27D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CD744779-D84C-4A3F-8151-1BA892EE796B}" name="Ingrés" totalsRowFunction="sum"/>
@@ -627,38 +741,50 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F8F6F14-CACE-4D29-ACF6-EA5358D9CC45}" name="Tabla2" displayName="Tabla2" ref="G2:J9" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F8F6F14-CACE-4D29-ACF6-EA5358D9CC45}" name="Tabla2" displayName="Tabla2" ref="G2:J9" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="G2:J9" xr:uid="{3F8F6F14-CACE-4D29-ACF6-EA5358D9CC45}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE1C2C8C-C2BE-4F7B-8E09-55F8AD976606}" name="Acorde 3" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{AE8773F4-D602-421C-91FE-4A396A729759}" name="Bajo" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{54941BB7-92C4-4E1D-85DF-D240A120A906}" name="Acorde 4" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{AF94B9CF-D253-471D-8F80-D57C8BA7A909}" name="Patrón" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{BE1C2C8C-C2BE-4F7B-8E09-55F8AD976606}" name="Acorde 3" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{AE8773F4-D602-421C-91FE-4A396A729759}" name="Bajo" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{54941BB7-92C4-4E1D-85DF-D240A120A906}" name="Acorde 4" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AF94B9CF-D253-471D-8F80-D57C8BA7A909}" name="Patrón" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B958FBBA-259C-4BFD-BB6A-8120E9427AA2}" name="Tabla3" displayName="Tabla3" ref="G12:K14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B958FBBA-259C-4BFD-BB6A-8120E9427AA2}" name="Tabla3" displayName="Tabla3" ref="G12:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2314DA57-1F08-402F-9396-A4B3FB3EE2AE}" name="Acorde"/>
-    <tableColumn id="2" xr3:uid="{3D7BE4EF-8702-4DC1-8DA1-AD8B34B74E5D}" name="1" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4125C2BB-65EF-402C-A629-A175B365D9EE}" name="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F7C3F633-4038-4183-A92B-E488209C8201}" name="5" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{BA53DA72-2D09-4C07-86A0-98811B8F481A}" name="7" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3D7BE4EF-8702-4DC1-8DA1-AD8B34B74E5D}" name="1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{4125C2BB-65EF-402C-A629-A175B365D9EE}" name="3" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{F7C3F633-4038-4183-A92B-E488209C8201}" name="5" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{BA53DA72-2D09-4C07-86A0-98811B8F481A}" name="7" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6AC57192-1E67-45CA-8EFC-DCE954DE3F55}" name="Tabla15" displayName="Tabla15" ref="B15:D21" totalsRowCount="1" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6AC57192-1E67-45CA-8EFC-DCE954DE3F55}" name="Tabla15" displayName="Tabla15" ref="B15:D21" totalsRowCount="1" headerRowBorderDxfId="9">
   <autoFilter ref="B15:D20" xr:uid="{6AC57192-1E67-45CA-8EFC-DCE954DE3F55}"/>
   <tableColumns count="3">
     <tableColumn id="3" xr3:uid="{7EAB856F-C910-426C-970E-EC0B536C3D60}" name="Establiment"/>
-    <tableColumn id="1" xr3:uid="{D178BE06-7AF7-4719-8CB4-95ADB9E78FF2}" name="Ingrés" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{5C6622AE-1861-48E9-B44D-19EE056C6514}" name="Càrrec" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D178BE06-7AF7-4719-8CB4-95ADB9E78FF2}" name="Ingrés" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5C6622AE-1861-48E9-B44D-19EE056C6514}" name="Càrrec" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{950B414E-ABB0-4DDD-9A92-FFFC0DDD68AC}" name="Tabla156" displayName="Tabla156" ref="B30:D37" totalsRowCount="1" headerRowBorderDxfId="4">
+  <autoFilter ref="B30:D36" xr:uid="{950B414E-ABB0-4DDD-9A92-FFFC0DDD68AC}"/>
+  <tableColumns count="3">
+    <tableColumn id="3" xr3:uid="{C13B49EC-030F-4AD2-AAC5-9411A253EACD}" name="Establiment"/>
+    <tableColumn id="1" xr3:uid="{68B6F8B5-32F0-4AAC-A748-D20BB2C37786}" name="Ingrés" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D96D36CA-5890-4D51-8C78-8C5F4AEA9AF9}" name="Càrrec" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -981,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7768563-7440-4184-B00C-C208FEBA8687}">
-  <dimension ref="B1:P25"/>
+  <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,14 +1488,96 @@
     <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D25" s="17"/>
     </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B29" s="15" t="str">
+        <f>"Saldo: "&amp;TEXT(Tabla156[[#Totals],[Ingrés]]-Tabla156[[#Totals],[Càrrec]],"0,00 ""€""")</f>
+        <v>Saldo: -214,05 €</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="15">
+        <v>0</v>
+      </c>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15">
+        <v>116.04</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15">
+        <v>16.78</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C37" s="15">
+        <f>SUBTOTAL(109,Tabla156[Ingrés])</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="15">
+        <f>SUBTOTAL(109,Tabla156[Càrrec])</f>
+        <v>214.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>